<commit_message>
Fixed issue with police_responses_monitor sheet
</commit_message>
<xml_diff>
--- a/docs/data-cleaning-requests/police_responses_monitor.xlsx
+++ b/docs/data-cleaning-requests/police_responses_monitor.xlsx
@@ -395,6 +395,11 @@
           <t>Today at approximately 11:30 Eastern Standard Time, protesters showed up to DePauw University yielding signs and Bibles, preaching that students who participated in "unholy behaviours" were going to hell. Eventually students took to responding against the protesters, at first in small numbers, then by the hundreds. Different groups on campus brought out gay pride flags and began chanting. During the protest, campus police shut down the surrounding streets. One student was handcuffed to prevent physical contact between the students and protesters, but no arrests were made. President Brian Casey was present at the protest.  The counter-protest group played loud music through speakers, chanted and waved gay-pride flags in an attempt to silence the Campus Ministry USA protesters. The group eventually grew to several dozen, including President Brian Casey and various members of DePauw's community, as well as state and Greencastle police. Then, one student threw a hot cup of coffee at the protesters. After this, sophomore Avery Nash approached the protesters. He was then detained by police as was Andrew Smith, assistant director for alumni engagement.</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Detain, Remove Individual Protesters, Force: Vague/Body, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -410,6 +415,11 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>In response to a rally demanding the removal of the state flag from the University of Mississippi campus (defending racist/racialized symbols), pro-flag supporters from the International Keystone Knights staged a counter-protest. They were escorted from the circle to the front of Fulton Chapel where they chanted and held Confederate flags. Chants bantered back and forth between students and the Knights. Knights member Shaun Winkler said, "Black lives don't matter." The Knights were escorted off campus after about 20 minutes.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Remove Individual Protesters</t>
         </is>
       </c>
     </row>
@@ -433,6 +443,11 @@
 The police presence was generally light, but thickened as the march continued, with about four dozen riot officers on the ground toward the end of the demonstration. There were a few tense standoffs between some more militant protesters shouting angrily at riot police officers who blocked access to certain streets. There was one arrest. After moving through downtown for nearly three hours, the march eventually ended with a hundred or so remaining protesters dispersing at the entrance of Berri metro station on Ste. Catherine St.</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Constrain, Arrest or Attempted</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -448,6 +463,11 @@
       <c r="C5" t="inlineStr">
         <is>
           <t>Black Lives Matter activists and allies gathered beneath the Martin Luther King Jr. statue at MacGregor Park to demand justice for fallen members of the black community following the recent police shootings of two Black men in the U.S. There was a time for open speaking where many volunteers shared their fears and urged the audience to push for change. As the protest marched toward University of Houston, upward of 80 people could be heard chanting along Calhoun Road and University Drive. Houston Police Department officers were present throughout the protest on foot, in squad cars and on horseback and received some hostility. At one point, HPD officers prevented protesters from moving toward Texas Spur 5 by lining up and forcing protesters to take another route through the University. Legal observers for the American Civil Liberties Union were present to document the proceedings of the protest and any misconduct between police and the demonstrators. From UH, Black Lives Matter: Houston and its supporters continued marching down Wheeler Avenue and past TDECU Stadium until they reached Texas Southern University. As protesters gathered at the historic Tiger Walk located at the university's entrance they heard a couple more speeches before the closing remarks.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Constrain, Monitor/Present</t>
         </is>
       </c>
     </row>
@@ -471,6 +491,11 @@
 Many event attendees expressed varying degrees of frustration with Security, as the scheduled start time for the talk passed, with no sign that they would be allowed to enter the room. At least one Security employee managing the crowd outside the Leacock Building reportedly told those in line that AMUSE members were causing the delay. In reality, the striking workers were engaged in a soft picket; that is, they had no intention of physically preventing anyone from entering the auditorium, and simply wished to inform those attending the talk that they would be crossing a picket line. Partly as a result of this, a great deal of misinformation seems to have been spread about the picket, resulting in a misplaced sense of outrage against AMUSE from some of the attendees. While many in the crowd expressed solidarity with them, others chanted “fuck your strike!” When Security eventually allowed students to enter the auditorium, students, who were aware there weren’t enough seats in Leacock 132 to accommodate everyone in line, began to push and shove to get in. AMUSE members appealed to attendees not to cross their picket line, but without much success, as Security personnel ushered people through the doors one by one, and hundreds of people pushed from behind to get in. When the auditorium met its capacity, Security closed the door, with many students still upset that they had been refused entry. It was announced that Leacock 26, down the hall, had been opened to accommodate overflow. Students again rushed to the door, with many pushing and shoving to get through. At least one student was hurt in the process. Ultimately, a representative of AMUSE’s parent union, Public Service Alliance of Canada, instructed the picketers to leave the building through a discreet back entrance for their own safety.</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Constrain, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -488,6 +513,11 @@
           <t>Evergreen State College students staged riots that lasted multiple days, beginning on the annual "Day of Absence,"  in response to an email sent by biology professor Bret Weinstein. During the riots, there were student confrontations with the campus chief of police, the college's president, and Professor Weinstein. Every year, students and staff of color leave campus for the day for the "Day of Absence" to highlight their vital and under appreciated roles. This year, however, organizers re-characterized the event's nature; Evergreen's Day of Absence program, designed for faculty, staff, and students of color, would happen on campus this year, while the program for allies would take place off campus. White students were thus discouraged from being on campus for the day. Opposing this change, Professor Weinstein emailed the entire staff stating, "There is a huge difference between a group or coalition deciding to voluntarily absent themselves from a shared space in order to highlight their vital and under-appreciated roles, and a group or coalition encouraging another group to go away. The first is a forceful call to consciousness which is, of course, crippling to the logic of oppression. The second is a show of force, and an act of oppression in and of itself." He declared that he would be on campus on the Day of Absence and encouraged others to reject this re-characterization of the annual event. During the protests staged in response to his email, students confronted Weinstein and disrupted his class. During the heated conversation, campus police and the county sheriffs were called in order to protect Weinstein. Students formed a protective ring around the students confronting Weinstein, but the police forced themselves through. Throughout the protests, participants also committed acts of vandalism and coercive pressure along with car-to-car hunting for allegedly racist staff and faculty, resulting in a brief closure of the campus. Rioters also called on Evergreen State College President George Bridges to fire Weinstein and order campus police to stand down. Some protesters even stormed Bridges' office, took over university spaces, and instituted "escorts". The President attempted to hold conversations with the outraged students, but he was met with shouted demands and mocking. Students ultimately occupied the President's office in order to conduct a meeting regarding their concerns and demands. The President eventually told campus police to "stand down" and listened to the student concerns. Following the riots, Evergreen reached a $500,000 settlement with the now former Professor Weinstein, and the college sanctioned about 80 student protesters for breaking the student code of conduct. Penalties for these students ranged from written warnings to suspensions.</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Force: Vague/Body, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -505,6 +535,11 @@
           <t>Students protested outside Carleton University's Richcraft Hall where a Board of Governors (BoG) meeting was being held. The students were protesting against the approval of the university's highly-debated sexual violence policy. Carleton increased security outside Richcraft Hall in response to the protest. Campus security also forcefully pushed student protesters out of the entrance of Richcraft Hall, and prevented students from climbing the overhang of the building.</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Force: Vague/Body</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -522,6 +557,11 @@
           <t>This is a one-day on-campus demonstration at Texas A &amp; M University in response to the rhetoric of 'alt-right' activist and white nationalist Richard Spencer, who spoke in the Memorial Student Center (MSC) about the movement. Members from the Texas A&amp;M community and around the state converged outside of Rudder Tower, Rudder Plaza and the MSC to express their views about the 'alt-right' movement. At the protest against Spencer's event, the student president of Texas A&amp;M Hillel said he was there to oppose white supremacy and neo-Nazism as a Jew whose grandparents were in the Holocaust and who also had many family members killed in the Holocaust. Notably, this article makes note of another protest titled "BTHOHate" that was taking place closer to where the above demonstration was taking place.</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Constrain, Force: Vague/Body</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -539,6 +579,11 @@
           <t>Members and supporters of the trans and non-binary community held a counter-protest to the “U of T Rally for Free Speech” in front of Sidney Smith Hall at the University of Toronto to disrupt what they viewed as hate speech. The free speech rally featured Lauren Southern, a conservative commentator with Rebel Media, and Professor Jordan Peterson, a U of T psychology professor who has made controversial statements on gender, and refused to use gender neutral pronouns. Peterson believes that Bill C-16 and associated Ontario Human Rights Commission policies place limitations on free speech in the interests of protecting peoples’ feelings (specifically with regards to using peoples’ proper pronouns). Trans and non-binary activists, along with members of the Black Liberation Collective, set up speakers behind Peterson and blasted white noise to drown out him and the speakers. The protesters also expressed their disagreement with Peterson's opinions, chanting “Shame! Shame! Shame!” The goal of the disruption was not to suppress anyone's free speech, but to make homophobic and transphobic statements a little harder to hear. The event also contained instances of violence and tension between some free speech rally attendees and individuals who came to counter-protest. Lauren Southern had glitter thrown at her and was shoved by a protester before a large scuffle ensued, during which her microphone was taken away. Campus and city police arrived to deal with both the crowd and isolated incidents of assault. They monitored the event and intervened in apparent escalating conflict. Partway through the rally, the fire alarm was pulled inside Sidney Smith Hall, causing students to evacuate the building and onto the street until the fire department came and gave the all clear. Following the event, the University of Toronto Students’ Union (UTSU) released a statement about inadequate response from campus police to alleged assaults against members of the trans community.</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Detain</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -556,6 +601,11 @@
           <t>Speaker Milo Yiannopoulos was to speak at UC Davis as part of his "The Dangerous Faggot Tour" with guest pharmaceutical executive Martin Shkreli. The event, hosted by the Davis College Republicans, was cancelled 30 minutes prior to Yiannopoulos taking the stage due to mass protests outside of the Sciences Lecture Hall venue. Prior to the 7 p.m. start time of the event, a crowd of hundreds gathered to protest it. Students at UC Davis blocked the entrance to a scheduled appearance by Yiannopoulos and former pharmaceutical executive Martin Shkreli. Students took issue with his rhetoric, which often featured racist, transphobic and anti-Semitic remarks. Many wore black handkerchiefs as face masks and held signs suggesting that Yiannopoulos and his fans were fascist and promoting hate speech. The protesters also chanted sayings such as "No Milo, no KKK, no fascist USA," "Say it loud say it clear, racists are not welcome here" and "This is what democracy looks like." Eggs were thrown during the protest and an ABC News cameraman reportedly had hot coffee thrown at him. One activist group stood in a line adjacent to the Sciences Lecture Hall holding signs that promoted love to minority groups. The UC Davis Police Department confiscated hammers that would be responsible for the protesters' violent and destructive actions of smashed windows and barricades being torn away.</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Arrest or Attempted</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -571,6 +621,11 @@
       <c r="C12" t="inlineStr">
         <is>
           <t>After a group of McGill University students began to occupy the sixth floor of the James Administration Building, a second group of students and faculty moved to protest outside of James, and gained entry to the front door despite attempts by security guards to secure the entrance. Once protesters gained entry to the lobby, guards blocked both the stairwell and elevators, and eventually shut off elevator service. These protesters then occupied the lobby of the building in solidarity with the sixth-floor occupiers. Both protests were in response to the administration's decision to invalidate a referendum that granted funding for CKUT and the Quebec Public Interest Research Group (QPIRG). In the referendum, students had voted to institute an in-person opt-out system for the fee levies paid to the groups, effectively making it harder to opt out. The sixth-floor occupiers said they would not leave until the administration met their two demands—that Deputy Provost Morton Mendelson resign, and that the administration ratify and recognize the QPIRG and CKUT fall referenda results. The sixth-floor occupation was thus framed as a "surprise resignation party" for Mendelson. Shortly after the occupations began, Provost Anthony Masi joined students in the lobby and responded to students’ inquiries regarding the invalidation of the vote; however, he was interrupted by a protester who explained that the occupiers upstairs had a very strict no-talking-to-administrators policy. At 3:30 p.m., students occupying the building in both the lobby and sixth floor were requested by Provost Anthony Masi to leave. Students in the lobby received a written notice stating that complaints will be addressed in accordance with the Code of Student Conduct and Disciplinary Procedures. Still, the solidarity occupiers remained. Around 5:45 p.m. students and faculty occupying the lobby sent a representative – Mob Squad member Amber Gross – to join negotiations between the sixth-floor occupiers and administration. They described her as a “solidarity ensurer,” stating that they hoped that they could participate without being labelled as occupiers. Throughout the occupation, McGill security prevented students in the lobby from using the elevators to reach the sixth floor, and after 9:30 p.m. security no longer allowed students to enter or bring food inside the building. This included not letting students re-enter who may have left the lobby for reasons such as finding a washroom. Around this time, wireless Internet was also disabled in the building. At the height of this solidarity occupation, there were nearly sixty students and faculty in the lobby, including a professor who brought his class to the lobby. Around 20 to 30 students stayed in the lobby overnight, despite being denied access to washrooms, food, or Internet. During the night, security guards filmed students sleeping. Additionally, a student who was seeking access to medication encountered resistance from security guards. The lobby protesters left the building around 11:20 a.m. the following day, after having spent 24 hours “partying” in solidarity with the sixth-floor occupiers. The lobby protesters ended their sit-in because they felt the space had become “unsafe.”</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Constrain, Instruct/Warn, Monitor/Present</t>
         </is>
       </c>
     </row>
@@ -598,6 +653,11 @@
 Note: Trump was not the headline issue of this protest</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Instruct/Warn, Force: 2+ Weapon Types, End Protest, "Breaking the Rules", Constrain, Arrest or Attempted, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -615,6 +675,11 @@
           <t>Several conservative groups and hundreds of Ann Coulter supporters gathered at Martin Luther King Jr. Civic Center Park in reaction to the cancellation of Ann Coulter's planned speech at UC Berkeley. More than 70 BPD officers were stationed throughout Martin Luther King Jr. Civic Center and along Telegraph and Shattuck avenues in anticipation of protests. BPD had planned for a "worst case scenario," according to Berkeley Police Department Lt. Andrew Rateaver. Coulter commented in an email to The Associated Press that she might "swing by to say hello," which helped to fuel tensions. Several protesters were arrested for assault and for refusing to remove masks. Students and groups of peaceful protesters gathered to talk to their opposition, calling for "discourse, not force. Police at one point formed a human wall in the street separating anti-Trump protesters from the park where pro-Trump groups were gathered. BPD also made five arrests in connection to the protest at Martin Luther King, Jr. Civic Center Park.</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Arrest or Attempted, Constrain, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -632,6 +697,11 @@
           <t>Protesters from The Revolutionary Communist Party were seen on campus standing on an American flag on the quad. Lou Downey, one of the protesters, said that security told him to stop stepping on the flag and to cease passing out literature. As students were handed fliers, the activists shouted "America was never great!" and "It's time for a revolution!" Downey pulled out a large American flag from his backpack and began standing on it until he was approached by the UCPD. A University spokesperson said that the UCPD asked the protester to move so that he would not block the public way.</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Instruct/Warn, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -649,6 +719,11 @@
           <t>Around 1,500 students marched through downtown Montreal wearing costumes as part of "La Grande Mascarade," a protest against Premier Jean Charest's planned tuition increases. In accordance with the masquerade theme of the protest, many participants wore colourful masks and costumes, drawing on the 18th and 19th century French tradition of the “charivari,” a moment when villagers donned costumes and masks and heckled a person in their home in order to criticize their conduct. A student protester described the event as "a symbolic protest." Some protesters also highlighted the masquerade theme as a response to Montreal Mayor Gérald Tremblay’s opposition to the use of masks in protests. The protest was split into four groups, and students followed routes through downtown Montreal that followed the Metro lines--blue, yellow, orange, and green--with each march representing a specific issue. About 600 protesters dressed in costumes and masks marched in the blue protest, which was called “Ensemble, bloquons la récupération!” The protest denounced the Quebec student federations the Fédération étudiante collégiale du Québec (FECQ) and the Fédération étudiante universitaire du Québec (FEUQ), and their non-representative stance during the student strike. Students with sparkly confetti threw handfuls at police cars and bystanders as they marched. A makeshift band marched among the blue line demonstrators including a tuba, drums and a trumpet. The blue protest also marched through the McGill campus and interrupted a mining conference that was taking place in a UQAM building. About 200 yellow demonstrators, also wearing masks, protested the issue of “syndicalisme jaune” – strikebreaking tactics employed by some students and student federations. Yellow demonstrators carried a effigy of Quebec Premier Jean Charest which participants took turns whipping or beating with flags. The march paused briefly outside the Loto-Québec building on Sherbrooke. Nine police officers blocked the building while the marchers chanted, some holding a hand over their right eye in reference to the injury suffered by Cégép St. Jerôme student Francis Grenier from a police stun grenade during a student protest. About 600 people took part in the orange march, which addressed the theme of the “ultraviolence” of the provincial government, denouncing “the violence of a government that refuses to negotiate and sends police instead.” Orange line protesters moved trash cans and construction signs to the middle of the streets, though many were moved back or set upright by students later in the march. Some vandalism also occurred, including the use of spray paint on a Université du Québec à Montréal building and on cars parked behind the police headquarters. Numbering several hundred students, the green march called for free education. Riot cops were scattered around the different march routes, watching over the Champlain Bridge and Service de police de la Ville de Montréal headquarters. Ten stood guard outside Premier Jean Charest’s office where a group of Concordia dance students organized a giant red square made of protesters. The four groups reconvened at Place-des-Arts after three hours of protesting. Many moved to the Université du Québec à Montréal (UQAM) sciences building for some spirited speeches, dancing and the burning of a Charest effigy. The SPVM reported three arrests, all charged for mischief.</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Constrain, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -666,6 +741,11 @@
           <t>Just after 5 p.m. Wednesday, CU Boulder administration ended a sit-in by Fossil Free CU protesters in the University Administrative Center that lasted nearly seven nights. Fossil Free CU is a student group on campus advocating for CU's divestment, or removal of investments, from the fossil fuel industry. They maintained the sit-in at the University Administrative Center since Thursday by rotating members in and out. Before settling into the UAC, they held sit-ins around campus last week, including at Old Main last Wednesday. They decided to move to the UAC to be more visible to the chancellor and his cabinet. CU Boulder police removed the possessions from the conference room where the group settled in for the protest. The students were not notified of the location of their belongings until 7:14 p.m., at which point they received an email detailing that they could be picked up at the UMC after showing photo identification.</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Instruct/Warn</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -684,6 +764,11 @@
 Spencer was one of the main perpetrators of this "Unite the Right" rally earlier in August in Charlottesville. In light of the way things went in Charlottesville at the Unite The Right Protests, which was Spencer's last public speech, hundreds of officers from Gainesville Police, Florida Highway Patrol, and Florida Fish and Wildlife Control were at University of Florida, lining the streets at times to create a barrier. Thousands of protesters gathering outside the Phillips Center at the University of Florida where Richard Spencer was slated to speak. Opposing white supremacy, protesters were peaceful as they drowned out Spencer's speech with boos. They also chartered a plane to scrawl the message "love will prevail" in the sky above the Phillips Center. The university spent $500,000 to ensure its students' safety. As well, Florida Gov. Rick Scott declared a state of emergency in advance of Spencer's speech and activated the Florida National Guard for the event. Only 400 students went to the actual speech at the University of Florida, most of whom only showed up in protest. Chants such as "go home" and "Nazis aren't welcome here" were yelled at Spencer, who responded by shouting that they were "morons."  A man wearing a shirt with several swastikas was punched in the face by a demonstrator. The offender, an unknown hooded man, scurried back into the mob.  At one point , three Texan, self-proclaimed white supremacists heckled anti-Spencer protesters with Nazi salutes and threats and proceeded to shoot at them. The bullet barely missed the crowd. Following the speech, they were charged with attempted murder for shooting at protestors,</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Arrest or Attempted, Constrain, Monitor/Present, Instruct/Warn</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -701,6 +786,11 @@
           <t>Protesters gathered outside Milo Yiannopoulos's speaking engagement at California State University - Fullerton in opposition to him. Eight people, including two members of the anti-fascist group Joe Hill Brigade, were arrested by Cal State Fullerton University Police in riot gear amid a swell of protests and provocations outside Milo Yiannopoulos' Tuesday evening speech in the Titan Student Union. Attendees to Yiannopoulos' "Troll Academy" tour stop filed out of the TSU to be greeted by a throng of demonstrators and hecklers, which had not decreased in size throughout the day, spurring confrontations that almost became altercations. Some attendees were chased off of Titan Walk. One female clad in riot gear was pursued by a crowd and University Police into the Pollak Library after throwing rocks and pepper-spraying people. The protester hid in the women's bathroom of the first floor as police cordoned off the elevators with batons and shields. Within moments, she was escorted out without her gear, hands bound by zip ties, to the applause of onlookers. University Police then ordered everyone to exit the library out of the east side. As students left the building, helicopters shined spotlights on the exodus and other parts of campus. Earlier in the day, riot-ready police units flanked the protesters on Titan Walk. The officers rushed the crowds with shields, detaining two members of the Joe Hill Brigade. The group's "medic" Murray, who did not give his last name, said the members have since been released without charges. "They hadn't done anything but treat people for pepper spray all night," Murray said. An altercation between protester Keyanne Celina, holding her 2-year-old child, and another woman occurred when the woman splashed coffee on Celina following a profanity-laced exchange. The fight prompted a shot of pepper spray into the surrounding crowd. The next few minutes were chaos as it disbanded. When the dust settled, one student was left on the ground, incapacitated by the pepper spray and covering her face in tears. To her aid came Murray, who said he treated three people for injuries that day. A left-wing activist, Murray also treated Yiannopoulos fan Elsa Aldeguer of the San Fernando Valley for pepper spray injuries sustained during the daytime altercation.</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Remove Individual Protesters, Arrest- Large Scale, Instruct/Warn, Constrain, Force: 2+ Weapon Types, Detain, Arrest or Attempted, Monitor/Present, Formal Accusation</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -718,6 +808,11 @@
           <t>Organized by the Société générale des étudiantes et étudiants du Collège de Maisonneuve, students participated in a march and occupation of the Fédération des cégeps building in Montreal. This protest action was part of a week of economic disruptions called for by the Coalition large de l’association pour une solidarité syndicale étudiante (CLASSE) in protest of the government's planned tuition increases. Protesters were not made aware of the protest action beforehand but were told the action was coded "green," meaning it was a low-risk action. The group of students, wearing red-squares, assembled at Henri-Julien park. At approximately 11:30 a.m., the students began marching through surrounding streets with one police car in front and one following. When the march reached the intersection of Crémazie and St. Denis, students began running. They ran towards the Fédération des cégeps building located at the corner of Crémazie and Berri. Students blocked the four entrances to the building, and initially a reported dozen students occupied the building. The students chanted and refused to move when asked by two police officers on the scene. Flyers stating the students’ demands were handed out. “We are occupying the Fédération des cégeps – the organization in charge of the direction of Quebec CEGEPs – to protest the budgetary reductions in the college network,” the flyer read in French. “Today, we ask that the Fédération des cégeps oppose the cuts in action and manage them in the interest of students and employees of the college network,” continued the flyer. Students occupied one half of the third floor of the building. Sticky notes and red squares were posted on the office walls, and the elevator doors were blocked. One note beside a drinking fountain read in French: “We’re thirsty for justice.” At 3:00 p.m., police tear gassed students as they ran into the nearby Jarry metro station.</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Instruct/Warn, Force: Vague/Body, Force: Weapon</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -735,6 +830,11 @@
           <t>About 100 people gathered at UC Berkeley's Crescent Lawn about noon for the "Berkeley Rally Against White Supremacy." The event was initially organized to protest the scheduled campus appearances of Milo Yiannopoulos, Ann Coulter and Steve Bannon, among others, for Free Speech Week. Organizers moved forward with the rally despite Free Speech Week's abrupt cancellation. At the rally, several attendees addressed the crowd, which was made up of UC Berkeley staff members, librarians, and local activist groups, including By Any Means Necessary (BAMN), Antifa, Socialist Alternative, Refuse Fascism and International Socialist Organization, Bay Area District. Several reporters from Infowars also attended the protest, but they were largely blocked off by protesters. Some protesters shouted at the Infowars staff members: "Bigot, bigot, out, out, out." The crowd, now 200 people, began to march towards campus about 1 p.m. As the protesters entered Wheeler Hall and students began leaving the Wheeler Auditorium, a fire alarm was pulled in the building, resulting in police officers organizing an evacuation of the area. Throughout the protest, police officers followed protesters to monitor the situation. At about 1:26 p.m, UCPD issued an alert that 200 people were occupying the steps and the inside of Wheeler Hall. By 1:40 p.m., about 100 protesters remained on the steps of the building, holding banners and chanting phrases, such as "They say get back, we say fight back." Some protesters inside Wheeler Hall hung a banner out the window that said "Cops off campus." The protesters issues largely revolved around white supremacy, the difference between speech and hate speech, as well as the militarization of police and police presence on campus.</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Arrest or Attempted, Formal Accusation, Instruct/Warn, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -752,6 +852,11 @@
           <t>Students from francophone universities and CEGEPs joined a Concordia student protest on March 27, marching through downtown Montreal in protest of the Charest government’s proposed tuition increases and in support of Amber Gross, a student who was allegedly hit by a Concordia security guard during a protest the day before. The demonstration began at Concordia's Hall building. From there, protesters marched through the downtown core. Approximately 150 to 200 students marched through the traffic on Sherbrooke St., gaining more protesters as the march continued. The march eventually entered McGill’s Humanities and Social Science Library and continued through the campus. Leaving McGill campus, the protesters then marched down René-Lévesque Blvd. At 2:00 p.m. they were joined by another protest group, organized by the Fédération des associations étudiantes du campus de l’Université de Montréal, at the corner of de Maisonneuve Blvd. W. and Guy St. There, protesters staged a sit-in at the intersection. The police had to intervene to regulate traffic and redirect the visibly angry motorists. They then marched up to Sherbrooke St., then down Mackay St. to Ste. Catherine St. W., to McGill College Ave. and back to Sherbrooke St. At least 2,000 protesters ended the march in front of Loto-Quebec’s offices on Sherbrooke Street, where a line of nine riot police were blocking the entrance. Students chanted and established a relaxed atmosphere by chatting with police officers.</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Constrain</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -769,6 +874,11 @@
           <t>Roughly 2,000 students marched through downtown Montreal in protest of the government's latest offer to Quebec's four main student associations regarding tuition hikes. The event for the demonstration was titled: “Demonstration against the government’s offer: freeze or strike.” Students marched peacefully for four hours until their numbers dwindled down to around 100. Police pushed the remaining marchers off the road as they walked north on Berri from Maisonneuve. An officer on the scene later confirmed to The Daily that the demonstration was never illegal.</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Constrain</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -786,6 +896,11 @@
           <t>A peaceful demonstration by hundreds of students and alumni began between Amos Eaton Hall and Lally Hall at Rensselaer Polytechnic Institute. The intended message of the protest was that "the overwhelming majority of the RPI community wants the Rensselaer Union restored to a student-run entity". Participants passionately shouted, "Save our Union!" protesters called for withholding donations. The protest originated outside of the fences enclosing the south side of campus.Thirty minutes into the protest, a portion of the fence was moved by demonstrators as they migrated onto the grass on the north side of the Voorhees Computing Center. The crowd later transitioned to the grass surrounding the walkway near EMPAC, where they continued to chant, display signs to alumni, and take turns speaking through a megaphone. Protesters broke through the fence erected by the university.</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Constrain</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -803,6 +918,11 @@
           <t>Hundreds of people gathered outside Indiana University's Franklin Hall to voice their concerns about controversial libertarian social scientist Charles Murray. Many students and faculty members were insulted IU gave Murray a platform to spread what they believed to be white-supremacist rhetoric. Some people banged pots an pants, and screamed into megaphones. There was a large police presence, seventy officers from IUPD, Bloomington Police Department and Indiana State Police were present in and around Franklin Hall to protect the protesters and the speaker. Some protesters chanted that Charles Murray is a white supremacist while others held up signs toward people walking into the hall. A protestor was taken into policy custody and released after other protestors started chanting Who do you serve? Who do you protect?" at the group of officers. One man in an orange bandanna raised a middle finger in one of the officer's faces.</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Constrain, Detain, Cooperate/Coordinate, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -818,6 +938,11 @@
       <c r="C26" t="inlineStr">
         <is>
           <t>Three student groups organized protests in response to a Ben Shapiro speaking event at the University of Utah. These groups included Students for a Democratic Society (SDS), Black Lives Matter and the Democratic Socialists of America, who combined in front of the Park Building for a rally in protest of Shapiro. As speakers addressed the crowd, counter-protesters gathered behind them chanting. After listening to several speakers, approximately 200 protesters marched toward the Social and Behavioral Science Building Auditorium, where the speech was being held. Police stood at the wings while security donning orange vests organized by SDS flanked the sides of marchers. As protesters arrived at the auditorium, police had set up barriers and stationed security around the building. More Shapiro supporters were waiting to stage a counter-protest. The two groups yelled back and forth, saying "All lives matter!" and "Black lives matter!" One protester said that they were protesting "because black lives have never mattered." The protesters opposing Shapiro also took a knee, paying homage to protesting NFL players. Many Shapiro protesters and supporters then separated into smaller groups. Some of the debates escalated into physical confrontations. In particular, a 17-year old girl protesting against Shapiro slapped a counter-protester who called her the n-word. In response, he hit her once on the side of her head, then on the top of her head as she collapsed, briefly rendering her unconscious. Police detained three individuals and took one into custody. Despite the violence, a tweet by the University's official account read "Tonight was a good example of how free speech should look on a university campus. Passionate people, nonviolently expressing their opinions."Another person was cited with disorderly conduct. Officers from multiple departments helped with security at the event.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Constrain, Detain, Formal Accusation, Arrest or Attempted</t>
         </is>
       </c>
     </row>
@@ -839,6 +964,11 @@
 Police detained three individuals and took one into custody. Another person was cited with disorderly conduct. Officers from multiple departments helped with security at the event.</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Remove Individual Protesters, Constrain, Detain, Formal Accusation</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -856,6 +986,11 @@
           <t>This event is protest white nationalists who were in support of White Nationalist Richard Spencer after he was invited to speak at the University of Florida. The white nationalists were counter-protesting protestors who were there to disrupt the speech. Spencer was one of the main perpetrators of this "Unite the Right" rally earlier in August in Charlottesville, and this was his first speech since then. In light of the way things went in Charlottesville at the Unite The Right Protests, there was a heavy police presence. The group of demonstrators gathered outside the Phillips Center in support of the presence of white nationalist Richard Spencer at the University of Florida, Randy Furniss, an unapologetic skinhead from Idaho, wandered over to the demonstration wearing a a t-shirt with several swastikas accompanied by red suspenders and a shaved head. Furniss was punched in the face by demonstrators. Three Texan, self-proclaimed white supremacists heckled anti-Spencer protesters with Nazi salutes and threats and proceeded to shoot at them. The bullet barely missed the crowd. The men have been arrested on charges of attempted homicide Two of the three men reportedly have connections to extremist white nationalist groups, and all three spoke with media in support of Spencer at the campus event prior to the attack. One Spencer supporter was assaulted by protesters. The man was wearing a white t-shirt with swastikas on it and red suspenders. Protesters hit the supporter at least once in the face, and he could later be seen with blood running down his chin. Florida Governor Rick Scott declared a state of emergency in the leadup to the speaking event, and many professors cancelled class in fear of placing their students in danger by asking them to come to class on the day of the rally.</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Arrest or Attempted, Formal Accusation, Instruct/Warn, Constrain, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -873,6 +1008,11 @@
           <t>About 300-500 counter protesters gathered at Carnegie Mellon University in response to a demonstration by the Westboro Baptist Church. The counter protest was referred to as "Time to Shine". The counter protesters filled the sidewalk and spilled over onto Forbes Ave, across the street from the WBC members. The two groups were separated by a line of police officers. One man rushed past officers and grabbed a sign from a Westboro Baptist member and attempted to rip it in half. He was arrested on charges of disorderly conduct. The counter-protesters chanted "hey ho, homophobia's got to go." A man playing the bagpipes stood right next to the WBC with the police separating them. The counter-protesters included community members, Christian church groups and CMU's LGBTQIA campus group. A Carlow student said she joined the counter-protest to support her friends who are part of Carlow's LGBTQIA+ community. Counter-protesters held signs that read "Christianity is not Westboro Baptist Church," "Free Prayer," "Love is love," "Trans rights and gay rights are human rights," and "Grads Together." One protester said she identifies as gay and said she came to "stand up for [her] people." They also displayed rainbow flags. Despite the rain, they held a rainbow flag and signs in what was essentially a pride rally. Pittsburgh police maintained a mostly calm relationship with the crowd for the duration of the event as well.</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Arrest or Attempted, Formal Accusation, Constrain, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -890,6 +1030,11 @@
           <t>A group of approximately 25 students, community leaders, and one professor held a march and demonstration at McGill University to demonstrate against austerity measures. The Parti Québécois (PQ) announced that it expects Quebec universities to cut $124 million from their cumulative operating budgets. The march began on campus at 3:30 p.m., going through the Leacock building and the Arts building, finally exiting through a side door onto James Square (also known as Community Square). Protesters held a banner that read “HMB en GGI.” At 3:45 p.m., 15 demonstrators entered the James Administration building through the side entrance and attempted to enter the meeting room on the third floor, where a Board of Governors (BoG) meeting was scheduled to take place at 4:00 p.m. The demonstrators were planning to present a motion to McGill’s BoG, for the administration of the University to go on unlimited general strike, create a working group to enforce the strike, and provide funds for strike-related initiatives. However, the protesters were denied access by security guards. Their presence also delayed the start of the meeting and caused the board to relocate to a different room. McGill’s Principal Heather Munroe-Blum later sent a message to the McGill community denouncing the budget cuts by the provincial government and stated that the administration will “take every measure necessary to persuade the government to withdraw these harmful and ill-timed cuts.”</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Constrain</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -907,6 +1052,11 @@
           <t>Around 100 protesters disrupted a lecture given by controversial author and activist Warren Farrell at the MacLeod auditorium at the University of Toronto on Friday night. The lecture, which included topics about men's rights and how males are disadvantaged in Western society, was hosted by the Canadian Association for Equality (CAFE). Protesters stood in front of the doors before the event, forming a barricade and blocking attendees from entering through the main doors of the auditorium and chanting slogans. They argued that his lecture is hate speech and causes a lot of damage to women particularly the ways in which he writes about consent and date rape. The lecture was delayed by the crowd of protestors, who had organized on Facebook through a coalition group calling themselves “U of T Students United Against Sexism.” About two dozen Toronto Police Service officers and U of T Campus Police were present to provide security.</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Detain, Monitor/Present, Arrest or Attempted</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -924,6 +1074,11 @@
           <t>At about 1 p.m., approximately 150 people gathered on Upper Sproul Plaza for a demonstration led by the Students of Color Solidarity Coalition. They were protesting against UC President Janet Napolitano who was visiting Berkeley on her tour of the UC system. Protesters expressed disapproval of Napolitano's history of deportation as the former Secretary of Homeland Security and of her nonacademic background. From Sproul Plaza, the group marched through campus and blocked the entrance of the Blum Center for Developing Economies, near another protest by the group BAMN. At this time, the two protests may have merged. At about 2:40 p.m., nine SCSC students entered the Blum Center, chaining the door and locking themselves inside. The protesters had three demands to the administration: that individuals inside the building receive amnesty, that Chancellor Nicholas Dirks call for Napolitano's resignation and that those in solidarity cancel classes Friday and "build a strike." They expressed they were willing to risk arrest and would not leave the building until their demands were met. Outside, some students spoke in megaphones to about 200 to 250 people at the height of the protest about 3 p.m. Some undergraduates who were in a listening conference with Napolitano in Sutardja Dai Hall walked out at about 3:30 p.m. to join the protest. At about 5:30 p.m., Chancellor Nicholas Dirks exited Sutardja Dai Hall. The protesters began to shout, claiming they deserved an audience with Dirks. Dirks briefly listened, then walked away. The protesters chanted, "Shame on you." Two UCPD officers arrived at 9 p.m. and warned protesters to leave the area. Although police did not taken any action to remove the protesters. As of 1 a.m., the demonstrations remained ongoing, although with only about 30 to 40 protesters outside the Blum Center for Developing Economies. The protest ended at 5 p.m. Friday.</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Instruct/Warn</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -941,6 +1096,11 @@
           <t>Divest Harvard was in the midst of Heat Week, a series of events taking place across Harvard campus to demand fossil fuel divestment and in protest of the appointment of new University Chief Financial Officer Thomas J. Hollister, who is a former oil executive. Roughly 15 Divest Harvard members blockaded three entrances to Massachusetts Hall at about 7:30 p.m. By 9 p.m., more protesters had joined them, bringing the total number of participants to at least 150 people. The group hung banners all around the building and pitched tarps and tents for their week of sleeping outside. University President Faust offered to meet with Divest Harvard members on Thursday on the condition they stop "disrupting university operations." The students continued their blockade, however, and did not meet with the president. The Harvard University Police Department arrested a member, though the student, Brett A. Roche '15, was not charged. The blockade is part of a planned weeklong protest the group has dubbed "Heat Week." The group continued their blockade until Friday, when "Heat Week" is scheduled to conclude.</t>
         </is>
       </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Formal Accusation, "Breaking the Rules", Monitor/Present, Arrest or Attempted</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -958,6 +1118,11 @@
           <t>The event was a march and rally, held at the University of Minnesota to oppose the Washington Redskins, specifically the team name and its racial connotations. Protesters marched across the University campus, converging on the TCF Bank Stadium, where the Minnesota Vikings were playing the Washington Redskins. The University of Minnesota partnered with the National Coalition Against Racism in Sports and Media, the Mille Lacs Band of Ojibwe, the Shakopee Mdewakanton Sioux tribe, and student groups, to help facilitate the rally.</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Constrain</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -975,6 +1140,11 @@
           <t>Demilitarize McGill, a group opposed to military research at the university, staged a silent protest during the annual Remembrance Day ceremony on McGill's campus. They held signs noting various facts that shed an unflattering light on the Canadian military and recent military operations-an attempt to disrupt what they saw as the narrative of "selective memory" implied by the ceremony. Messages on the posters also touched on sexual assault in the military, weapons manufacturing, civilian casualty statistics, and torture. During the demonstration, police officers approached the protesters and asked them to leave. After the demonstrators refused to comply, the police did not press the issue and left the scene.  The protest angered many users on social media, who called it disrespectful. Demilitarize McGill also protested at Remembrance Day ceremonies in previous years. Demilitarize McGill later addressed the enraged reaction to the protest, saying that angry people lend credibility to Demilitarize McGill's basic claim about Remembrance Day.</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Instruct/Warn</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -992,6 +1162,11 @@
           <t>Student and community activists began occupying Wheeler Hall after a general assembly meeting on Sproul Plaza in the aftermath of a UC Board of Regents committee voting 7-2 to approve a tuition increase plan. Occupiers posted a 13-point list of demands on a wall that included stopping fee hikes, adding more students to the UC Board of Regents, creating a corporate tax to fund education and holding public dialogue on tuition increases. Graffiti was found in the building with messages such as "Fuck the UC Regents," "Kill Napolitano" and "Struggle is forever." The occupation lasted for 7 days.</t>
         </is>
       </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Instruct/Warn, "Breaking the Rules"</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1007,6 +1182,11 @@
       <c r="C37" t="inlineStr">
         <is>
           <t>On February 9, Occupy Cal protesters set up six tents on the steps of UC Berkeley's Sproul Hall, to protest against tuition increases and state funding cuts and mark the three month anniversary of the controversial Nov. 9 Occupy campus protest. About 25 individuals were present when the tents were originally erected at around 1:15 p.m. Shortly after the tents went up, two UCPD officers requested they be removed, but protesters refused, saying they were not in violation of campus policy. That evening, Dean of Students Jonathan Poullard and campus police officers addressed the protesters. Poullard said they were not authorized to camp on university property and those who remained in continued violation of campus policy may be subject to disciplinary action. As of about 9 p.m., about 25 protesters and five tents remained on the steps and a dispersal order had not been given. Demonstrators said they intended to stay overnight, but that a dispersal order from UCPD would prompt either a vote to brave police intervention or to leave the choice up to individual protesters. On the first day of the occupation, the student protesters held a general assembly where they voted on decisions. Thursday night continued peacefully, interrupted only by a visit from one UCPD officer at 3 a.m. Students passed the time with frisbee games, soccer, singing and storytelling. As protesters were setting up a rally on the steps at noon Friday, Assistant Director in the Center for Student Leadership Jeff Woods informed them that they would not be able to use speakers because they did not receive approval from the campus administration to reserve the space. Friday and Saturday evenings saw little incident, protesters said. Around 3 p.m. Sunday, 30 to 40 protesters gathered on the steps for a potluck, and seven tents remained set up. So far, UCPD had not issued a dispersal order to the protesters, and they planned to continue the occupation. Claire Holmes, associate vice chancellor for public affairs, said the University had someone out there every few hours to check up on the situation. On Monday, protesters decided shortly before midnight to temporarily move to the steps in front of UC Berkeley's largest library in an effort to draw students' attention toward library cuts. University administration and campus police continued to monitor the situation, as they claimed the tents were still in violation of campus policy in the new location. On the following Friday, the encampment ended after eight days when seven student and 11 nonstudent protesters were told that "camping and lodging on campus is against university policy and state law." They left peacefully after being detained and identified by the police. Eleven of the protesters were given a stay-away order for seven days, and 10 of the encampment's 13 tents were taken into police custody. Campus administrators ordered the police action after Occupy protesters did not respond to UCPD's daily warnings that they would be cited if they did not leave.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Instruct/Warn, Monitor/Present, "Breaking the Rules", Detain, Formal Accusation, End Protest</t>
         </is>
       </c>
     </row>
@@ -1032,6 +1212,11 @@
 They were met by counter-protestors at the rotunda and the march turned violent near the statue of Thomas Jefferson north of the Rotunda, leading to physical altercations and the use of pepper spray. The group left the university's grounds when police arrived and declared the gathering an unlawful assembly.  The following week, University of Virginia police said they obtained arrest warrants for a white nationalist in connection with crimes committed during this protest march. This man stated that he would turn himself in to authorities and acknowledged he had pepper-sprayed a counter-protester but insisted he was defending himself.</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Formal Accusation, Arrest or Attempted, End Protest</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1049,6 +1234,11 @@
           <t>This event was a small counter-protest of around 20 people to a white nationalist march at the University of Virginia.  After Charlottesville City Council voted to remove a statue of confederate general Robert E. Lee, white nationalists began planning a Unite the Right rally scheduled to take place on Aug 12, 2017. The evening prior to the rally on Aug 11th, about 250 torch-bearing White Nationalists, Neo-Nazis and other supporters held a torch-lit march through the University of Virginia campus which caused some UVA community members and students to organize a counter-protest against them. The purpose was to fight for freedom and equality against the threatening presence of the white supremacists. The small group of counter protestors stood in a circle around the statue of Thomas Jefferson where they were surrounded by over 300 protesters carrying torches came down the steps and surrounded them. The anti-racism protesters held a banner reading "VA Students Act Against White Supremacy." Clashes between the groups followed; Gorcenski said she was doused in lighter fluid and maced, and was harassed for her gender - some of the torchbearers yelled, "You're not a woman." Police then intervened and declared an unlawful assembly. Chris Cantwell, who was a scheduled speaker for the Unite the Right rally, was later arrested and charged in the incident.</t>
         </is>
       </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Arrest or Attempted, Formal Accusation, Monitor/Present</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1064,6 +1254,11 @@
       <c r="C40" t="inlineStr">
         <is>
           <t>Approximately 100 students demonstrated around Concordia University, marching between buildings while carrying out “anti-capitalistes” chants, picketing and disrupting classes, and gathering support for their cause against austerity measures by the provincial government. Students entered the Library building and disrupted the library by chanting, then moved to Hall, where the protesters began picketing against ongoing classes. During a cross-listed class between SCPA, which had a strike mandate to protest against austerity measures by the provincial government, and Political Science, which didn’t have a strike mandate, students disrupted the class. Some students and protesters were seen shouting at one another, almost coming to blows. The situation became tense when the majority of class attendees did not leave. Instead they confronted the picketers on their willingness to disturb a class mostly attended by political science students whose Political Science Student Association (PSSA) was set to vote on the strike that Monday night. Concordia Student Union (CSU) President Benjamin Prunty, who was present at the picket said that he considered such classes shared between striking and non-striking student associations as a “predictable kind of grey area.”. The disruption eventually ended when the professor left. Concordia security officials filmed the protest and police were present as protesters entered the Hall building, although no arrests were made. Protesters then moved to the EV and MB buildings on Guy St., and then to the Fine Arts building, but it was mostly empty. The group then moved onto the streets, where police attempted to stop the demonstration. Protesters continued and ended inside the EV building, at which point most of the students dispersed, with some remaining at a table organized by the Fine Arts Student Alliance. The protesters were enforcing the strike motions of several Concordia student associations that are currently on strike against austerity, including the Fine Arts Student Alliance (FASA), Women’s Studies Student Association (WSSA), Undergraduate Students of Philosophy Association (SoPHiA), Geography Undergraduate Student Society (GUSS), and the School of Community and Public Affairs Student Association (SCPASA).</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Monitor/Present, Instruct/Warn</t>
         </is>
       </c>
     </row>

</xml_diff>